<commit_message>
add data outbreak 2
</commit_message>
<xml_diff>
--- a/norovirus/relevantData.xlsx
+++ b/norovirus/relevantData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lihel\Documents\master\so24\case_studies\CaseStudiesLifeSciences\norovirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C928664-48BD-49F8-990E-C0B07DB9B00D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF03BAE-9B82-46E6-AB73-3E8ABD31264D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2940" yWindow="2940" windowWidth="15390" windowHeight="9442" xr2:uid="{02D1537A-C68A-4117-A4F6-E02188D431B9}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" activeTab="1" xr2:uid="{02D1537A-C68A-4117-A4F6-E02188D431B9}"/>
   </bookViews>
   <sheets>
     <sheet name="outbreak11" sheetId="1" r:id="rId1"/>
+    <sheet name="outbreak2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
   <si>
     <t>time</t>
   </si>
@@ -426,7 +427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C71414F3-59BC-4D03-BC5C-71C8F0B84F4A}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -539,4 +540,67 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72F9606B-F8DB-44EC-B4FC-30B362640094}">
+  <dimension ref="A1:B6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>